<commit_message>
Updated some tracking sheets and added examples with a key
</commit_message>
<xml_diff>
--- a/houseTrkSheet.xlsx
+++ b/houseTrkSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\rba-col-dc01\RedirectedFolders\CCrowe\Desktop\areatracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F3A351E-A896-4B34-8EF8-9635C25D65A7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC825401-1CC5-4B07-98A0-437B52D61300}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12915" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Street</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>Total Knocked:                                    Total Contacts:                               Total PHO:</t>
-  </si>
-  <si>
-    <t>Rent?</t>
   </si>
 </sst>
 </file>
@@ -481,36 +478,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G84"/>
+  <dimension ref="A1:F84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="8.875" customWidth="1"/>
-    <col min="3" max="4" width="5.375" customWidth="1"/>
-    <col min="5" max="5" width="7" customWidth="1"/>
-    <col min="6" max="6" width="5.375" customWidth="1"/>
-    <col min="7" max="7" width="26.625" customWidth="1"/>
+    <col min="3" max="3" width="5.375" customWidth="1"/>
+    <col min="4" max="4" width="7" customWidth="1"/>
+    <col min="5" max="5" width="5.375" customWidth="1"/>
+    <col min="6" max="6" width="26.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>7</v>
       </c>
+      <c r="E1" s="5"/>
       <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -518,742 +514,659 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
-      <c r="G57" s="2"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
-      <c r="G59" s="2"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
-      <c r="G60" s="3"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
-      <c r="G61" s="2"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
-      <c r="G62" s="3"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
-      <c r="G63" s="2"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
-      <c r="G64" s="3"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
-      <c r="G65" s="2"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
-      <c r="G66" s="3"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
-      <c r="G67" s="2"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
-      <c r="G68" s="3"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
-      <c r="G69" s="2"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
-      <c r="G70" s="3"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
-      <c r="G71" s="2"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
-      <c r="G72" s="3"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
-      <c r="G73" s="2"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
-      <c r="G74" s="3"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
-      <c r="G75" s="2"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
-      <c r="G76" s="3"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
-      <c r="G77" s="2"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
-      <c r="G78" s="3"/>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
-      <c r="G79" s="2"/>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
-      <c r="G80" s="3"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
-      <c r="G81" s="2"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
       <c r="D82" s="4"/>
       <c r="E82" s="4"/>
       <c r="F82" s="4"/>
-      <c r="G82" s="4"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
         <v>8</v>
       </c>
@@ -1262,22 +1175,20 @@
       <c r="D83" s="8"/>
       <c r="E83" s="8"/>
       <c r="F83" s="8"/>
-      <c r="G83" s="8"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="9"/>
       <c r="B84" s="9"/>
       <c r="C84" s="9"/>
       <c r="D84" s="9"/>
       <c r="E84" s="9"/>
       <c r="F84" s="9"/>
-      <c r="G84" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="A83:G84"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A83:F84"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>